<commit_message>
Splicing database access into OrderManager
</commit_message>
<xml_diff>
--- a/WorkBot/main/backend/ordering/OrderFiles/A.L. George/A.L. George_Triphammer_20250704.xlsx
+++ b/WorkBot/main/backend/ordering/OrderFiles/A.L. George/A.L. George_Triphammer_20250704.xlsx
@@ -451,135 +451,135 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>75157</t>
+          <t>sku</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Essentia Water</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>16.50</t>
+          <t>cost_per</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>66.00</t>
+          <t>total_cost</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>74602</t>
+          <t>sku</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Evian 1L</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>22.00</t>
+          <t>cost_per</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>22.00</t>
+          <t>total_cost</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>75112</t>
+          <t>sku</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Fiji Water 1L</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>16.50</t>
+          <t>cost_per</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>33.00</t>
+          <t>total_cost</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>75101</t>
+          <t>sku</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fiji Water 500ml</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>18.50</t>
+          <t>cost_per</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>18.50</t>
+          <t>total_cost</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>77802</t>
+          <t>sku</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ithaca Soda - Ginger Beer</t>
+          <t>name</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>quantity</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>28.75</t>
+          <t>cost_per</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>28.75</t>
+          <t>total_cost</t>
         </is>
       </c>
     </row>

</xml_diff>